<commit_message>
ligne changement selon document initiale
</commit_message>
<xml_diff>
--- a/TP1/revue_code/revue_code_MohamadHujaij.xlsx
+++ b/TP1/revue_code/revue_code_MohamadHujaij.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamad\Documents\TP1-420-5GP-BB\TP1\revue_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9AA2A5-0CFA-40A5-9BC5-639278E2F93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6016459A-F735-40FD-A05E-0656BB823321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{A048998D-8A6E-437B-863F-D5E4D7A0533E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
   <si>
     <t>PROJET</t>
   </si>
@@ -126,12 +126,6 @@
     <t xml:space="preserve">Le nom de variable"index" n'est pas significatif. </t>
   </si>
   <si>
-    <t xml:space="preserve">Le nom de variable"i" n'est pas significatif. </t>
-  </si>
-  <si>
-    <t>De 50 à 102</t>
-  </si>
-  <si>
     <t>Manque de commentaires qui assurent la compréhension du code.</t>
   </si>
   <si>
@@ -147,30 +141,12 @@
     <t>Correction</t>
   </si>
   <si>
-    <t>8 à 17</t>
-  </si>
-  <si>
-    <t>33 à 42</t>
-  </si>
-  <si>
     <t>Mettre ce bloc de code dans une fonction.</t>
   </si>
   <si>
-    <t>8 à 111</t>
-  </si>
-  <si>
     <t>Mettre dans le main (incluant les fonctions).</t>
   </si>
   <si>
-    <t>52 à 56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60 à 102 </t>
-  </si>
-  <si>
-    <t>104 à 107</t>
-  </si>
-  <si>
     <t>La variable fichier est en français alors que la majorité des variables sont en anglais.</t>
   </si>
   <si>
@@ -184,6 +160,27 @@
   </si>
   <si>
     <t>Billet</t>
+  </si>
+  <si>
+    <t>8 à 16</t>
+  </si>
+  <si>
+    <t>7 à 110</t>
+  </si>
+  <si>
+    <t>33 à 41</t>
+  </si>
+  <si>
+    <t>De 50 à 101</t>
+  </si>
+  <si>
+    <t>51 à 55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61 à 101 </t>
+  </si>
+  <si>
+    <t>103 à 106</t>
   </si>
 </sst>
 </file>
@@ -601,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EF6733-6B20-4ADE-95E8-4F31CB65AA28}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -713,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>26</v>
@@ -722,27 +719,27 @@
         <v>27</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
-        <f t="shared" ref="A13:A33" si="0">A12+1</f>
+        <f t="shared" ref="A13:A32" si="0">A12+1</f>
         <v>2</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -753,16 +750,16 @@
         <v>3</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -773,16 +770,16 @@
         <v>4</v>
       </c>
       <c r="B15" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -793,7 +790,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>26</v>
@@ -802,7 +799,7 @@
         <v>23</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -813,16 +810,16 @@
         <v>6</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -833,7 +830,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="6">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>20</v>
@@ -842,7 +839,7 @@
         <v>28</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -853,16 +850,16 @@
         <v>8</v>
       </c>
       <c r="B19" s="6">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -873,7 +870,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="6">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>20</v>
@@ -882,7 +879,7 @@
         <v>29</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -893,16 +890,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="6">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -913,16 +910,16 @@
         <v>11</v>
       </c>
       <c r="B22" s="6">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -933,16 +930,16 @@
         <v>12</v>
       </c>
       <c r="B23" s="6">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -959,10 +956,10 @@
         <v>20</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -972,17 +969,17 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B25" s="6">
-        <v>49</v>
+      <c r="B25" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -993,16 +990,16 @@
         <v>15</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1012,17 +1009,17 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>42</v>
+      <c r="B27" s="6">
+        <v>57</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1033,16 +1030,16 @@
         <v>17</v>
       </c>
       <c r="B28" s="6">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1052,17 +1049,17 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B29" s="6">
-        <v>60</v>
+      <c r="B29" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1072,17 +1069,17 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>43</v>
+      <c r="B30" s="6">
+        <v>59</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1093,16 +1090,16 @@
         <v>20</v>
       </c>
       <c r="B31" s="6">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1112,40 +1109,20 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B32" s="6">
-        <v>91</v>
+      <c r="B32" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="5">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>